<commit_message>
signed off all testing
</commit_message>
<xml_diff>
--- a/Test Plan.xlsx
+++ b/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganda\Documents\GitHub\Software-Engineering-Principles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AC3591-5344-4EF2-9266-4BC27513501B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8781346-FD06-4345-A9B5-65BD8323A57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="92">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>cannot report a review</t>
+  </si>
+  <si>
+    <t>Sufiyan, Isaac</t>
   </si>
 </sst>
 </file>
@@ -423,14 +426,14 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -718,7 +721,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,15 +758,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -780,7 +783,9 @@
         <v>85</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -797,7 +802,9 @@
         <v>85</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -814,7 +821,9 @@
         <v>85</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -831,7 +840,9 @@
         <v>85</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -848,7 +859,9 @@
         <v>85</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -865,7 +878,9 @@
         <v>85</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -882,7 +897,9 @@
         <v>85</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -899,7 +916,9 @@
         <v>85</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -916,7 +935,9 @@
         <v>85</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -933,7 +954,9 @@
         <v>85</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -950,7 +973,9 @@
         <v>85</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -967,18 +992,20 @@
         <v>85</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -995,7 +1022,9 @@
         <v>85</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1012,7 +1041,9 @@
         <v>85</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1029,7 +1060,9 @@
         <v>85</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -1044,7 +1077,9 @@
         <v>85</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1061,7 +1096,9 @@
         <v>85</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -1078,7 +1115,9 @@
         <v>85</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1095,18 +1134,20 @@
         <v>85</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1123,7 +1164,9 @@
         <v>85</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -1140,7 +1183,9 @@
         <v>85</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -1157,7 +1202,9 @@
         <v>85</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -1174,41 +1221,43 @@
         <v>85</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="5">
         <v>24</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7" t="s">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="7"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="5">
         <v>25</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7" t="s">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="7"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -1225,7 +1274,9 @@
         <v>85</v>
       </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -1242,7 +1293,9 @@
         <v>85</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="G31" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -1259,7 +1312,9 @@
         <v>85</v>
       </c>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -1276,18 +1331,20 @@
         <v>85</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1304,7 +1361,9 @@
         <v>85</v>
       </c>
       <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
@@ -1321,26 +1380,28 @@
         <v>85</v>
       </c>
       <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="A37" s="5">
         <v>32</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G37" s="7"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -1357,7 +1418,9 @@
         <v>85</v>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
+      <c r="G38" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
@@ -1374,18 +1437,20 @@
         <v>85</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
@@ -1402,7 +1467,9 @@
         <v>85</v>
       </c>
       <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
@@ -1419,7 +1486,9 @@
         <v>85</v>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
+      <c r="G42" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
@@ -1436,18 +1505,20 @@
         <v>85</v>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
@@ -1464,7 +1535,9 @@
         <v>85</v>
       </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="G45" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
@@ -1481,7 +1554,9 @@
         <v>85</v>
       </c>
       <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
@@ -1498,140 +1573,142 @@
         <v>85</v>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
+      <c r="A48" s="5">
         <v>41</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7" t="s">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G48" s="7"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+      <c r="A49" s="5">
         <v>42</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7" t="s">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G49" s="7"/>
+      <c r="G49" s="5"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+      <c r="A50" s="5">
         <v>43</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7" t="s">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E50" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G50" s="7"/>
+      <c r="G50" s="5"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+      <c r="A51" s="5">
         <v>44</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7" t="s">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G51" s="7"/>
+      <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+      <c r="A52" s="5">
         <v>45</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7" t="s">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="E52" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G52" s="7"/>
+      <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+      <c r="A53" s="5">
         <v>46</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7" t="s">
+      <c r="B53" s="5"/>
+      <c r="C53" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G53" s="7"/>
+      <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+      <c r="A54" s="5">
         <v>47</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7" t="s">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G54" s="7"/>
+      <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2">

</xml_diff>

<commit_message>
testing and design done
</commit_message>
<xml_diff>
--- a/Test Plan.xlsx
+++ b/Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganda\Documents\GitHub\Software-Engineering-Principles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8781346-FD06-4345-A9B5-65BD8323A57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759915D5-97F4-4C84-83F5-D0886573CD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="93">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>Sufiyan, Isaac</t>
+  </si>
+  <si>
+    <t>Isaac, Isaac</t>
   </si>
 </sst>
 </file>
@@ -720,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +844,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -860,7 +863,7 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,7 +882,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>